<commit_message>
# UPDATE : เพิ่ม U5 (27/11/2017)
</commit_message>
<xml_diff>
--- a/TestID/StudentList/studentListcs284.xlsx
+++ b/TestID/StudentList/studentListcs284.xlsx
@@ -23,28 +23,28 @@
     <t>Name Lastname</t>
   </si>
   <si>
-    <t>Homework Score</t>
-  </si>
-  <si>
-    <t>Quiz Score</t>
-  </si>
-  <si>
-    <t>Midterm Score</t>
-  </si>
-  <si>
-    <t>Final Score</t>
-  </si>
-  <si>
-    <t>HomeworkNet Score</t>
-  </si>
-  <si>
-    <t>QuizNet Score</t>
-  </si>
-  <si>
-    <t>MidtermNet Score</t>
-  </si>
-  <si>
-    <t>FinalNet Score</t>
+    <t>HW_Score</t>
+  </si>
+  <si>
+    <t>Q_Score</t>
+  </si>
+  <si>
+    <t>Midterm_Score</t>
+  </si>
+  <si>
+    <t>Final_Score</t>
+  </si>
+  <si>
+    <t>HMN_Score</t>
+  </si>
+  <si>
+    <t>QN_Score</t>
+  </si>
+  <si>
+    <t>MidtermN_Score</t>
+  </si>
+  <si>
+    <t>FinalN_Score</t>
   </si>
   <si>
     <t>Grade</t>
@@ -208,6 +208,10 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="2" max="2" width="15.625" customWidth="true"/>
+    <col min="3" max="3" width="39.0625" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -258,7 +262,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="E2" t="n">
         <v>0.0</v>
@@ -267,10 +271,10 @@
         <v>0.0</v>
       </c>
       <c r="G2" t="n">
-        <v>30.0</v>
+        <v>0.0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="I2" t="n">
         <v>0.0</v>
@@ -279,7 +283,7 @@
         <v>0.0</v>
       </c>
       <c r="K2" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="L2"/>
     </row>
@@ -339,7 +343,7 @@
         <v>0.0</v>
       </c>
       <c r="G4" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="H4" t="n">
         <v>0.0</v>
@@ -351,7 +355,7 @@
         <v>0.0</v>
       </c>
       <c r="K4" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="L4"/>
     </row>
@@ -375,7 +379,7 @@
         <v>0.0</v>
       </c>
       <c r="G5" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="H5" t="n">
         <v>0.0</v>
@@ -387,7 +391,7 @@
         <v>0.0</v>
       </c>
       <c r="K5" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="L5"/>
     </row>
@@ -411,7 +415,7 @@
         <v>0.0</v>
       </c>
       <c r="G6" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
       <c r="H6" t="n">
         <v>0.0</v>
@@ -423,7 +427,7 @@
         <v>0.0</v>
       </c>
       <c r="K6" t="n">
-        <v>30.0</v>
+        <v>0.0</v>
       </c>
       <c r="L6"/>
     </row>
@@ -546,7 +550,7 @@
         <v>20</v>
       </c>
       <c r="D10" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="E10" t="n">
         <v>0.0</v>
@@ -555,10 +559,10 @@
         <v>0.0</v>
       </c>
       <c r="G10" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
       <c r="H10" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="I10" t="n">
         <v>0.0</v>
@@ -567,7 +571,7 @@
         <v>0.0</v>
       </c>
       <c r="K10" t="n">
-        <v>30.0</v>
+        <v>0.0</v>
       </c>
       <c r="L10"/>
     </row>
@@ -699,7 +703,7 @@
         <v>0.0</v>
       </c>
       <c r="G14" t="n">
-        <v>60.0</v>
+        <v>0.0</v>
       </c>
       <c r="H14" t="n">
         <v>0.0</v>
@@ -711,7 +715,7 @@
         <v>0.0</v>
       </c>
       <c r="K14" t="n">
-        <v>30.0</v>
+        <v>0.0</v>
       </c>
       <c r="L14"/>
     </row>
@@ -1563,7 +1567,7 @@
         <v>0.0</v>
       </c>
       <c r="G38" t="n">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
       <c r="H38" t="n">
         <v>0.0</v>
@@ -1575,7 +1579,7 @@
         <v>0.0</v>
       </c>
       <c r="K38" t="n">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="L38"/>
     </row>

</xml_diff>

<commit_message>
#Update UI (27/11/2017 : 22:07)
</commit_message>
<xml_diff>
--- a/TestID/StudentList/studentListcs284.xlsx
+++ b/TestID/StudentList/studentListcs284.xlsx
@@ -262,7 +262,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="n">
-        <v>20.0</v>
+        <v>10.0</v>
       </c>
       <c r="E2" t="n">
         <v>0.0</v>
@@ -271,10 +271,10 @@
         <v>0.0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="H2" t="n">
-        <v>20.0</v>
+        <v>7.0</v>
       </c>
       <c r="I2" t="n">
         <v>0.0</v>
@@ -283,7 +283,7 @@
         <v>0.0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="L2"/>
     </row>

</xml_diff>